<commit_message>
Updated bioenergetics in multispecies input file
</commit_message>
<xml_diff>
--- a/data/hake_multisp_220307.xlsx
+++ b/data/hake_multisp_220307.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E24D7BD-5DB7-1E41-93D9-F7224DE8FA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD43E0C-3B22-5A4F-9483-95283469256D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="20840" windowWidth="25600" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="33460" windowHeight="20380" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,24 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UobsWtAge!$A$1:$I$201</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="511">
   <si>
     <t>Number</t>
   </si>
@@ -1574,6 +1586,9 @@
   <si>
     <t>ATF_survey</t>
   </si>
+  <si>
+    <t>Arrowtooth flounder</t>
+  </si>
 </sst>
 </file>
 
@@ -1968,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -20644,115 +20659,157 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>138</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>140</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>142</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>144</v>
       </c>
       <c r="B6">
-        <v>0.1190094</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>146</v>
       </c>
       <c r="B7">
-        <v>-0.46023779999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-0.46</v>
+      </c>
+      <c r="C7">
+        <v>-0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>148</v>
       </c>
       <c r="B8">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+      <c r="C8">
+        <v>2.4969999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>150</v>
       </c>
       <c r="B9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>20.512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>151</v>
       </c>
       <c r="B10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>152</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>153</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
       <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13">
         <v>17</v>
       </c>
     </row>

</xml_diff>